<commit_message>
adding fastq filenames back to 159
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_159.xlsx
+++ b/fastqFiles/fastq_159.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t xml:space="preserve">libraryDate</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">[128]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_6_sequence_37C_CO2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_6_sequence_CHX_30C.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s_6_sequence_CHX_37C_CO2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -162,12 +171,14 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,6 +252,9 @@
       <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>14</v>
+      </c>
       <c r="H3" s="0" t="n">
         <v>1</v>
       </c>
@@ -264,6 +278,9 @@
       <c r="E4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" s="0" t="n">
         <v>1</v>
       </c>
@@ -286,6 +303,9 @@
       </c>
       <c r="E5" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>1</v>

</xml_diff>